<commit_message>
Adicionando Vídeo aos arquivos
</commit_message>
<xml_diff>
--- a/Data/Temp/Filmes.xlsx
+++ b/Data/Temp/Filmes.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://t2cconsultoria365-my.sharepoint.com/personal/mithel_medeiros_t2cgroup_com_br/Documents/Documentos/Avaliação/2024/prj_FilmesMarvel_Avaliacao/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_AD4D361C20488DEA4E38A0A4D41D6B885ADEDD8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E77FA3C7-5E75-487F-8C9A-15BB073A29D2}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_AD4D361C20488DEA4E38A0A4D41D6B885ADEDD8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{538E36FC-3013-45F8-B368-611DB06C0EFC}"/>
   <x:bookViews>
-    <x:workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Export" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Export" sheetId="2" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="162913"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <x:si>
     <x:t>Título do Filme</x:t>
   </x:si>
@@ -46,7 +46,10 @@
     <x:t>Iron Man</x:t>
   </x:si>
   <x:si>
-    <x:t>0</x:t>
+    <x:t>94</x:t>
+  </x:si>
+  <x:si>
+    <x:t>91</x:t>
   </x:si>
   <x:si>
     <x:t>SUCESSO</x:t>
@@ -55,40 +58,31 @@
     <x:t>-</x:t>
   </x:si>
   <x:si>
+    <x:t>Thor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>77</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Iron Man 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72</x:t>
+  </x:si>
+  <x:si>
+    <x:t>71</x:t>
+  </x:si>
+  <x:si>
     <x:t>The Incredible Hulk</x:t>
   </x:si>
   <x:si>
-    <x:t>Iron Man 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Captain America: The First Avenger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Avengers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Iron Man 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thor: The Dark World</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Captain America: The Winter Soldier</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Guardians of the Galaxy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Avengers: Age of Ultron</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ant-Man</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Captain America: Civil War</x:t>
+    <x:t>67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -107,8 +101,9 @@
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
+      <x:b/>
       <x:sz val="11"/>
-      <x:color theme="1"/>
+      <x:color theme="0"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
       <x:scheme val="minor"/>
@@ -121,15 +116,21 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
     </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor theme="4"/>
+        <x:bgColor theme="4"/>
+      </x:patternFill>
+    </x:fill>
   </x:fills>
-  <x:borders count="1">
+  <x:borders count="4">
     <x:border>
       <x:left/>
       <x:right/>
@@ -137,35 +138,88 @@
       <x:bottom/>
       <x:diagonal/>
     </x:border>
+    <x:border>
+      <x:left style="thin">
+        <x:color theme="4" tint="0.39997558519241921"/>
+      </x:left>
+      <x:right/>
+      <x:top style="thin">
+        <x:color theme="4" tint="0.39997558519241921"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color theme="4" tint="0.39997558519241921"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top style="thin">
+        <x:color theme="4" tint="0.39997558519241921"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color theme="4" tint="0.39997558519241921"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
+    <x:border>
+      <x:left/>
+      <x:right style="thin">
+        <x:color theme="4" tint="0.39997558519241921"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color theme="4" tint="0.39997558519241921"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color theme="4" tint="0.39997558519241921"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="10" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="9">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellXfs>
-  <x:cellStyles count="2">
+  <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <x:cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </x:cellStyles>
-  <x:dxfs count="2">
-    <x:dxf>
-      <x:font>
-        <x:color theme="1"/>
-      </x:font>
-    </x:dxf>
-    <x:dxf>
-      <x:font>
-        <x:color theme="1"/>
-      </x:font>
-      <x:numFmt numFmtId="9" formatCode="0%"/>
-    </x:dxf>
-  </x:dxfs>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -180,20 +234,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela2" displayName="Tabela2" ref="A1:E2" totalsRowShown="0">
-  <x:autoFilter ref="A1:E2"/>
-  <x:tableColumns count="5">
-    <x:tableColumn id="1" name="Título do Filme" dataDxfId="0"/>
-    <x:tableColumn id="2" name="Tomatometer" dataDxfId="0"/>
-    <x:tableColumn id="3" name="Audience" dataDxfId="1"/>
-    <x:tableColumn id="4" name="Status" dataDxfId="0"/>
-    <x:tableColumn id="5" name="Motivo Status" dataDxfId="0"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,39 +498,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{3C86B49D-AA3F-4B73-B452-31C677B3B70D}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:E1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B2" sqref="B2 B2:C1048576"/>
+      <x:selection activeCell="B8" sqref="B8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="22.425781" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="15.285156" style="1" customWidth="1"/>
-    <x:col min="3" max="3" width="12.285156" style="1" customWidth="1"/>
-    <x:col min="4" max="4" width="12.285156" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="15.425781" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="24.570312" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.285156" style="5" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="15.710938" style="5" customWidth="1"/>
+    <x:col min="4" max="4" width="15.140625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="20.285156" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="0" t="s">
+      <x:c r="A1" s="6" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s">
+      <x:c r="B1" s="7" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="0" t="s">
+      <x:c r="C1" s="7" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="0" t="s">
+      <x:c r="D1" s="7" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
+      <x:c r="E1" s="8" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
@@ -498,230 +538,78 @@
       <x:c r="A2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="B2" s="5" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C2" s="1" t="s">
-        <x:v>6</x:v>
+      <x:c r="C2" s="5" t="s">
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B3" s="5" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C3" s="5" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
         <x:v>9</x:v>
-      </x:c>
-      <x:c r="B3" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C3" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B4" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C4" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B4" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C4" s="5" t="s">
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B5" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C5" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B5" s="5" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C5" s="5" t="s">
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5">
-      <x:c r="A6" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B6" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C6" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="A7" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B7" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C7" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
-      <x:c r="A8" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B8" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C8" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="A9" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B9" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C9" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5">
-      <x:c r="A10" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B10" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C10" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B11" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C11" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5">
-      <x:c r="A12" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B12" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C12" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5">
-      <x:c r="A13" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B13" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C13" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5">
-      <x:c r="A14" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B14" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C14" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E14" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
+      <x:c r="B8" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
-  <x:tableParts count="1">
-    <x:tablePart r:id="rId1"/>
-  </x:tableParts>
+  <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>